<commit_message>
Added Else in Get Transaction data state
</commit_message>
<xml_diff>
--- a/Data/Input/Data.xlsx
+++ b/Data/Input/Data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <x:si>
     <x:t>No</x:t>
   </x:si>
@@ -62,67 +62,91 @@
     <x:t>O +ve</x:t>
   </x:si>
   <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\50886.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>William Middlebrooks</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Purchase </x:t>
+  </x:si>
+  <x:si>
+    <x:t>A +ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\28438.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sarah Neighbors</x:t>
+  </x:si>
+  <x:si>
+    <x:t>B +ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\22137.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Henry Hunter</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Marketing </x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\23915.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daniel Padillo</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Finance </x:t>
+  </x:si>
+  <x:si>
+    <x:t>AB +ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\39636.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sharon Becerra</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\67564.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Leah Gibbs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Exception Occured DOJ is missing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rosie Pica</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A -ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\84162.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robert Conner</x:t>
+  </x:si>
+  <x:si>
+    <x:t>O -ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System Exception:File "H:\UiPath2023versions\IDCardGeneration\Data\Input\GeneratedIDCards\46141.docx" already exists. Please check "Replace existing" or specify a file that doesn't exist.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Angelia Cartee</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sales </x:t>
+  </x:si>
+  <x:si>
+    <x:t>AB -ve</x:t>
+  </x:si>
+  <x:si>
     <x:t>Successfully ID Card Created</x:t>
-  </x:si>
-  <x:si>
-    <x:t>William Middlebrooks</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Purchase </x:t>
-  </x:si>
-  <x:si>
-    <x:t>A +ve</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sarah Neighbors</x:t>
-  </x:si>
-  <x:si>
-    <x:t>B +ve</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Henry Hunter</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Marketing </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daniel Padillo</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Finance </x:t>
-  </x:si>
-  <x:si>
-    <x:t>AB +ve</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sharon Becerra</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Leah Gibbs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Exception Occured DOJ is missing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rosie Pica</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A -ve</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Robert Conner</x:t>
-  </x:si>
-  <x:si>
-    <x:t>O -ve</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Angelia Cartee</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Sales </x:t>
-  </x:si>
-  <x:si>
-    <x:t>AB -ve</x:t>
   </x:si>
   <x:si>
     <x:t>Marie Burgess</x:t>
@@ -663,7 +687,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H3" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -671,7 +695,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C4" s="1" t="s">
         <x:v>11</x:v>
@@ -683,10 +707,10 @@
         <x:v>44634</x:v>
       </x:c>
       <x:c r="F4" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H4" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -694,10 +718,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C5" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D5" s="1" t="n">
         <x:v>23915</x:v>
@@ -709,7 +733,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H5" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -717,10 +741,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C6" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D6" s="1" t="n">
         <x:v>39636</x:v>
@@ -729,10 +753,10 @@
         <x:v>44636</x:v>
       </x:c>
       <x:c r="F6" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="H6" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -740,10 +764,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C7" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D7" s="1" t="n">
         <x:v>67564</x:v>
@@ -755,7 +779,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H7" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -763,7 +787,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
         <x:v>7</x:v>
@@ -776,7 +800,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H8" s="6" t="s">
-        <x:v>22</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -784,10 +808,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D9" s="1" t="n">
         <x:v>84162</x:v>
@@ -796,10 +820,10 @@
         <x:v>44580</x:v>
       </x:c>
       <x:c r="F9" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H9" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -807,10 +831,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D10" s="1" t="n">
         <x:v>46141</x:v>
@@ -819,10 +843,10 @@
         <x:v>44612</x:v>
       </x:c>
       <x:c r="F10" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H10" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -830,10 +854,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D11" s="1" t="n">
         <x:v>94396</x:v>
@@ -842,10 +866,10 @@
         <x:v>44613</x:v>
       </x:c>
       <x:c r="F11" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H11" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -853,10 +877,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D12" s="1" t="n">
         <x:v>56066</x:v>
@@ -868,7 +892,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H12" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -876,7 +900,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C13" s="1" t="s">
         <x:v>7</x:v>
@@ -888,10 +912,10 @@
         <x:v>44615</x:v>
       </x:c>
       <x:c r="F13" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="H13" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -899,7 +923,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>33</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C14" s="1" t="s">
         <x:v>7</x:v>
@@ -912,7 +936,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H14" s="6" t="s">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -920,10 +944,10 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D15" s="4" t="s"/>
       <x:c r="E15" s="2">
@@ -933,7 +957,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="H15" s="6" t="s">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -941,20 +965,20 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
-        <x:v>36</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D16" s="1" t="n">
         <x:v>13457</x:v>
       </x:c>
       <x:c r="E16" s="4" t="s"/>
       <x:c r="F16" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H16" s="6" t="s">
-        <x:v>22</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.75">
@@ -962,7 +986,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
-        <x:v>37</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
         <x:v>7</x:v>
@@ -977,7 +1001,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="H17" s="6" t="s">
-        <x:v>9</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>